<commit_message>
✅ Corregir número de estudiantes: 42 (no 43)
Correcciones:
- adaptar_datos_itc.py: Filtrar fila vacía con promedios
- ITC-RESULTADOS-ICFES-2025-ADAPTADO.xlsx: Regenerado con 42 estudiantes
- README.md: Actualizar todas las referencias de 43 a 42 estudiantes

Análisis:
- Archivo original tenía 43 filas
- Fila 42 contenía promedios (sin nombre de estudiante)
- Total estudiantes reales: 42

Estadísticas actualizadas:
- Promedio Global: 334
- Mediana: 338
- Rango: 250-409
</commit_message>
<xml_diff>
--- a/ITC-RESULTADOS-ICFES-2025-ADAPTADO.xlsx
+++ b/ITC-RESULTADOS-ICFES-2025-ADAPTADO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2686,43 +2686,6 @@
         <v>269</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>11A</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
-        <v>1000000042</v>
-      </c>
-      <c r="H44" t="n">
-        <v>66</v>
-      </c>
-      <c r="I44" t="n">
-        <v>75.66666666666667</v>
-      </c>
-      <c r="J44" t="n">
-        <v>62</v>
-      </c>
-      <c r="K44" t="n">
-        <v>65.28571428571429</v>
-      </c>
-      <c r="L44" t="n">
-        <v>62.04761904761905</v>
-      </c>
-      <c r="M44" t="n">
-        <v>334.0952380952381</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>